<commit_message>
corriger horaire à Simon
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfrechette\workspace\techinfo\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCBAE0E-8C77-4101-8356-50F940D493C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE36B93-93B4-3247-91D0-A10C8B3167EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -726,17 +726,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF1DC5-63E0-A14F-8B6A-86AB73F394B2}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -762,7 +762,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -788,7 +788,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -814,7 +814,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -840,7 +840,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -866,7 +866,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -892,7 +892,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -918,7 +918,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -944,7 +944,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -970,7 +970,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -996,7 +996,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -1984,9 +1984,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>18</v>
@@ -2010,9 +2010,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>26</v>
@@ -2036,9 +2036,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>19</v>
@@ -2062,9 +2062,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>20</v>
@@ -2088,7 +2088,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
correction horaire + ajout numéro groupe
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE36B93-93B4-3247-91D0-A10C8B3167EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AA0F12-0166-4C46-B655-40BE734A9DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="101">
   <si>
     <t>Lundi</t>
   </si>
@@ -191,33 +191,15 @@
     <t>Gestion d'un poste</t>
   </si>
   <si>
-    <t>Outils informatiques (2)</t>
-  </si>
-  <si>
-    <t>Outils informatiques (1)</t>
-  </si>
-  <si>
     <t>D204</t>
   </si>
   <si>
     <t>Frederick</t>
   </si>
   <si>
-    <t>Programmation 1 (2)</t>
-  </si>
-  <si>
-    <t>Programmation 1 (1)</t>
-  </si>
-  <si>
     <t>Simon</t>
   </si>
   <si>
-    <t>Fonctionnement de l'ordinateur (1)</t>
-  </si>
-  <si>
-    <t>Fonctionnement de l'ordinateur (2)</t>
-  </si>
-  <si>
     <t>Logiciel de gestion</t>
   </si>
   <si>
@@ -336,6 +318,27 @@
   </si>
   <si>
     <t>13:05</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>SFC</t>
+  </si>
+  <si>
+    <t>Outils informatiques</t>
+  </si>
+  <si>
+    <t>Programmation 1</t>
+  </si>
+  <si>
+    <t>Fonctionnement de l'ordinateur</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -724,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF1DC5-63E0-A14F-8B6A-86AB73F394B2}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +739,7 @@
     <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -744,7 +747,7 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
@@ -759,10 +762,13 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -770,7 +776,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -785,10 +791,13 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -796,7 +805,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -811,10 +820,13 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -822,7 +834,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -837,10 +849,13 @@
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -848,7 +863,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -863,10 +878,13 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -874,7 +892,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
@@ -889,10 +907,13 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -900,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -915,10 +936,13 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -926,7 +950,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
@@ -941,10 +965,13 @@
         <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -952,7 +979,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -967,10 +994,13 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -978,7 +1008,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
@@ -993,10 +1023,13 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1004,7 +1037,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -1019,10 +1052,13 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
@@ -1045,10 +1081,13 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1056,7 +1095,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -1068,13 +1107,16 @@
         <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1082,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
@@ -1094,13 +1136,16 @@
         <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1108,7 +1153,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
@@ -1120,13 +1165,16 @@
         <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1182,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2">
         <v>2</v>
@@ -1149,10 +1197,13 @@
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1211,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -1175,44 +1226,50 @@
         <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D18" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
         <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
@@ -1221,24 +1278,27 @@
         <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2">
         <v>2</v>
@@ -1247,50 +1307,56 @@
         <v>35</v>
       </c>
       <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
         <v>36</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>12</v>
       </c>
-      <c r="H20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="H21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -1302,47 +1368,53 @@
         <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
@@ -1357,41 +1429,47 @@
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
         <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>93</v>
@@ -1403,50 +1481,56 @@
         <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>87</v>
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>79</v>
       </c>
       <c r="H27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -1455,76 +1539,85 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" t="s">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -1533,21 +1626,24 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>93</v>
@@ -1559,180 +1655,201 @@
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D33" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
         <v>44</v>
       </c>
       <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="2">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
         <v>48</v>
       </c>
-      <c r="G33" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" s="2">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" t="s">
-        <v>85</v>
-      </c>
-      <c r="H34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="2">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>86</v>
+      <c r="G35" t="s">
+        <v>79</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="I35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D36" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
         <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D37" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E37" t="s">
         <v>49</v>
       </c>
       <c r="F37" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="H37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I37">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D38" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
       </c>
       <c r="F38" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="H38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
@@ -1741,24 +1858,27 @@
         <v>49</v>
       </c>
       <c r="F39" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="G39" t="s">
         <v>37</v>
       </c>
       <c r="H39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D40" s="2">
         <v>2</v>
@@ -1767,637 +1887,770 @@
         <v>49</v>
       </c>
       <c r="F40" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
         <v>49</v>
       </c>
       <c r="F41" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" t="s">
+        <v>97</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>70</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" t="s">
         <v>50</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="G43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" t="s">
+        <v>70</v>
+      </c>
+      <c r="I43">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="2">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" t="s">
-        <v>55</v>
-      </c>
-      <c r="G42" t="s">
-        <v>5</v>
-      </c>
-      <c r="H42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="2">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>54</v>
-      </c>
-      <c r="F43" t="s">
-        <v>56</v>
-      </c>
-      <c r="G43" t="s">
-        <v>37</v>
-      </c>
-      <c r="H43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C44" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D44" s="2">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="G45" t="s">
         <v>37</v>
       </c>
       <c r="H45" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D46" s="2">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="G46" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H46" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D47" s="2">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F47" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="G47" t="s">
         <v>37</v>
       </c>
       <c r="H47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D48" s="2">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G48" t="s">
+        <v>37</v>
+      </c>
+      <c r="H48" t="s">
+        <v>71</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="2">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" t="s">
+        <v>98</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>71</v>
+      </c>
+      <c r="I49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
         <v>33</v>
       </c>
-      <c r="G48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="2">
-        <v>2</v>
-      </c>
-      <c r="E49" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" t="s">
-        <v>58</v>
-      </c>
-      <c r="G49" t="s">
-        <v>5</v>
-      </c>
-      <c r="H49" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="2">
-        <v>2</v>
-      </c>
-      <c r="E50" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" t="s">
-        <v>59</v>
-      </c>
       <c r="G50" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="H50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="I50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>29</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D52" s="2">
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F52" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>99</v>
+      </c>
+      <c r="G53" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="2">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>99</v>
+      </c>
+      <c r="G54" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" t="s">
+        <v>72</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>6</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="2">
-        <v>2</v>
-      </c>
-      <c r="E53" t="s">
-        <v>57</v>
-      </c>
-      <c r="F53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G53" t="s">
-        <v>61</v>
-      </c>
-      <c r="H53" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>32</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D54" s="2">
-        <v>2</v>
-      </c>
-      <c r="E54" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" t="s">
-        <v>62</v>
-      </c>
-      <c r="G54" t="s">
-        <v>88</v>
-      </c>
-      <c r="H54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>10</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D55" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G55" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="H55" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="H56" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="I56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D57" s="2">
         <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F57" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G57" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="H57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="2">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" t="s">
+        <v>58</v>
+      </c>
+      <c r="G59" t="s">
+        <v>83</v>
+      </c>
+      <c r="H59" t="s">
+        <v>73</v>
+      </c>
+      <c r="I59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="2">
+      <c r="B60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="2">
         <v>3</v>
       </c>
-      <c r="E58" t="s">
-        <v>63</v>
-      </c>
-      <c r="F58" t="s">
-        <v>66</v>
-      </c>
-      <c r="G58" t="s">
-        <v>5</v>
-      </c>
-      <c r="H58" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>32</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="2">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>63</v>
-      </c>
-      <c r="F59" t="s">
-        <v>45</v>
-      </c>
-      <c r="G59" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="2">
-        <v>2</v>
-      </c>
       <c r="E60" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F60" t="s">
         <v>60</v>
       </c>
       <c r="G60" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="H60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D61" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F61" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="G61" t="s">
         <v>12</v>
       </c>
       <c r="H61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D62" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G62" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="H62" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>29</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D63" s="2">
         <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G63" t="s">
         <v>12</v>
       </c>
       <c r="H63" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>93</v>
       </c>
       <c r="D64" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F64" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="G64" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" t="s">
+        <v>75</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D65" s="2">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>63</v>
+      </c>
+      <c r="F65" t="s">
+        <v>64</v>
+      </c>
+      <c r="G65" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" t="s">
+        <v>74</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="2">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F66" t="s">
+        <v>64</v>
+      </c>
+      <c r="G66" t="s">
         <v>11</v>
       </c>
-      <c r="H64" t="s">
-        <v>80</v>
+      <c r="H66" t="s">
+        <v>74</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modification horaire, grille et autre
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522471EE-ACC8-DF4E-BE13-E2FFFB85C4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F788D169-6BDD-3B4C-9B50-8F9F857C5AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="95">
   <si>
     <t>Lundi</t>
   </si>
@@ -128,21 +128,12 @@
     <t>Mardi</t>
   </si>
   <si>
-    <t>16:15</t>
-  </si>
-  <si>
-    <t>CFTV</t>
-  </si>
-  <si>
     <t>Jeudi</t>
   </si>
   <si>
     <t>ACD</t>
   </si>
   <si>
-    <t>Commission des études</t>
-  </si>
-  <si>
     <t>Carine</t>
   </si>
   <si>
@@ -308,9 +299,6 @@
     <t>16:05</t>
   </si>
   <si>
-    <t>9:05</t>
-  </si>
-  <si>
     <t>13:05</t>
   </si>
   <si>
@@ -333,12 +321,6 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>Nouveau</t>
   </si>
 </sst>
 </file>
@@ -727,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF1DC5-63E0-A14F-8B6A-86AB73F394B2}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,7 +729,7 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
@@ -762,10 +744,10 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -776,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -791,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -805,7 +787,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -820,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -834,7 +816,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -849,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -863,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -878,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -892,7 +874,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
@@ -907,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -921,7 +903,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -936,7 +918,7 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -944,13 +926,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
@@ -962,10 +944,10 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -979,7 +961,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -994,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -1008,7 +990,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
@@ -1023,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1037,7 +1019,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -1052,7 +1034,7 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1066,7 +1048,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
@@ -1081,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1089,16 +1071,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1107,126 +1089,126 @@
         <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
         <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" t="s">
-        <v>98</v>
+        <v>71</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
       </c>
-      <c r="G15" t="s">
-        <v>79</v>
-      </c>
       <c r="H15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" t="s">
-        <v>98</v>
+        <v>71</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="I16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1234,57 +1216,57 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D18" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
         <v>35</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" t="s">
         <v>94</v>
-      </c>
-      <c r="G18" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1292,173 +1274,173 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I20" t="s">
-        <v>98</v>
+        <v>64</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D21" s="2">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" t="s">
-        <v>98</v>
+        <v>64</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" t="s">
-        <v>77</v>
+        <v>40</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D25" s="2">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I25">
         <v>2</v>
@@ -1466,16 +1448,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
         <v>41</v>
@@ -1487,50 +1469,50 @@
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>67</v>
-      </c>
-      <c r="I27" t="s">
-        <v>98</v>
+        <v>65</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -1539,27 +1521,27 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>79</v>
+        <v>44</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" t="s">
-        <v>98</v>
+        <v>65</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
@@ -1571,13 +1553,13 @@
         <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1588,25 +1570,25 @@
         <v>18</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H30" t="s">
-        <v>67</v>
-      </c>
-      <c r="I30">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="I30" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1614,112 +1596,112 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H31" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="I31" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
         <v>46</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="2">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>44</v>
       </c>
       <c r="F32" t="s">
         <v>47</v>
       </c>
-      <c r="G32" t="s">
-        <v>12</v>
+      <c r="G32" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="H32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>20001</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F33" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H33" t="s">
-        <v>68</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2">
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F34" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="H34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I34">
         <v>2</v>
@@ -1727,129 +1709,129 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D35" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="H35" t="s">
-        <v>68</v>
-      </c>
-      <c r="I35" t="s">
-        <v>98</v>
+        <v>66</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="G36" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>69</v>
-      </c>
-      <c r="I36" t="s">
-        <v>98</v>
+        <v>66</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="2">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>78</v>
+      <c r="G37" t="s">
+        <v>11</v>
       </c>
       <c r="H37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I37">
-        <v>20001</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D38" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F38" t="s">
-        <v>76</v>
-      </c>
-      <c r="G38" t="s">
-        <v>77</v>
+        <v>47</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="H38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I38" t="s">
-        <v>98</v>
+        <v>66</v>
+      </c>
+      <c r="I38">
+        <v>10001</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
@@ -1858,13 +1840,13 @@
         <v>49</v>
       </c>
       <c r="F39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G39" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I39">
         <v>2</v>
@@ -1872,13 +1854,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D40" s="2">
         <v>2</v>
@@ -1887,13 +1869,13 @@
         <v>49</v>
       </c>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="H40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -1901,13 +1883,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D41" s="2">
         <v>2</v>
@@ -1916,13 +1898,13 @@
         <v>49</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -1930,13 +1912,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
@@ -1945,13 +1927,13 @@
         <v>49</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I42">
         <v>2</v>
@@ -1959,39 +1941,39 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D43" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" t="s">
         <v>49</v>
       </c>
       <c r="F43" t="s">
-        <v>50</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>51</v>
+        <v>92</v>
+      </c>
+      <c r="G43" t="s">
+        <v>34</v>
       </c>
       <c r="H43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I43">
-        <v>10001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>83</v>
@@ -2000,16 +1982,16 @@
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G44" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I44">
         <v>2</v>
@@ -2017,57 +1999,57 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F45" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="G45" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="H45" t="s">
-        <v>70</v>
-      </c>
-      <c r="I45">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="I45" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D46" s="2">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G46" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -2075,28 +2057,28 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D47" s="2">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G47" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I47">
         <v>2</v>
@@ -2104,28 +2086,28 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D48" s="2">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G48" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -2133,28 +2115,28 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D49" s="2">
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H49" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I49">
         <v>2</v>
@@ -2162,86 +2144,86 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D50" s="2">
         <v>2</v>
       </c>
       <c r="E50" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" t="s">
         <v>52</v>
       </c>
-      <c r="F50" t="s">
-        <v>33</v>
-      </c>
-      <c r="G50" t="s">
-        <v>79</v>
-      </c>
       <c r="H50" t="s">
-        <v>70</v>
-      </c>
-      <c r="I50" t="s">
-        <v>98</v>
+        <v>68</v>
+      </c>
+      <c r="I50">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
       </c>
       <c r="E51" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" t="s">
         <v>53</v>
       </c>
-      <c r="F51" t="s">
-        <v>97</v>
-      </c>
       <c r="G51" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="H51" t="s">
-        <v>71</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="I51" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D52" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F52" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="G52" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H52" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I52">
         <v>2</v>
@@ -2249,28 +2231,28 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D53" s="2">
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F53" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -2278,144 +2260,144 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D54" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="G54" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="H54" t="s">
-        <v>71</v>
-      </c>
-      <c r="I54">
-        <v>2</v>
+        <v>69</v>
+      </c>
+      <c r="I54" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D55" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F55" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="H55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F56" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="G56" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>71</v>
-      </c>
-      <c r="I56" t="s">
-        <v>98</v>
+        <v>69</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D57" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F57" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G57" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="H57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D58" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F58" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="G58" t="s">
         <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -2423,57 +2405,57 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D59" s="2">
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F59" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G59" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>72</v>
-      </c>
-      <c r="I59" t="s">
-        <v>98</v>
+        <v>70</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D60" s="2">
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F60" t="s">
         <v>60</v>
       </c>
       <c r="G60" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H60" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -2481,175 +2463,30 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D61" s="2">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F61" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H61" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D62" s="2">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>61</v>
-      </c>
-      <c r="F62" t="s">
-        <v>54</v>
-      </c>
-      <c r="G62" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" t="s">
-        <v>73</v>
-      </c>
-      <c r="I62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>29</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63" s="2">
-        <v>3</v>
-      </c>
-      <c r="E63" t="s">
-        <v>61</v>
-      </c>
-      <c r="F63" t="s">
-        <v>62</v>
-      </c>
-      <c r="G63" t="s">
-        <v>12</v>
-      </c>
-      <c r="H63" t="s">
-        <v>73</v>
-      </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" s="2">
-        <v>3</v>
-      </c>
-      <c r="E64" t="s">
-        <v>61</v>
-      </c>
-      <c r="F64" t="s">
-        <v>54</v>
-      </c>
-      <c r="G64" t="s">
-        <v>7</v>
-      </c>
-      <c r="H64" t="s">
-        <v>73</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D65" s="2">
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>100</v>
-      </c>
-      <c r="F65" t="s">
-        <v>63</v>
-      </c>
-      <c r="G65" t="s">
-        <v>12</v>
-      </c>
-      <c r="H65" t="s">
-        <v>99</v>
-      </c>
-      <c r="I65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D66" s="2">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s">
-        <v>100</v>
-      </c>
-      <c r="F66" t="s">
-        <v>63</v>
-      </c>
-      <c r="G66" t="s">
-        <v>11</v>
-      </c>
-      <c r="H66" t="s">
-        <v>99</v>
-      </c>
-      <c r="I66">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajustement horaire + stage 2025
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AA80FC-F949-4B40-85BC-D993109DBC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D7EADB-2613-F64E-A3EC-D6DE72AC3611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="97">
   <si>
     <t>Lundi</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -712,7 +718,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2475,7 +2481,7 @@
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="F61" t="s">
         <v>60</v>
@@ -2484,7 +2490,7 @@
         <v>12</v>
       </c>
       <c r="H61" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -2504,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="F62" t="s">
         <v>60</v>
@@ -2513,7 +2519,7 @@
         <v>11</v>
       </c>
       <c r="H62" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="I62">
         <v>1</v>

</xml_diff>

<commit_message>
changement horaire ER et AO
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AA594E-7E53-D148-AA76-228C86D8B8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A761EAB3-2E12-8344-95ED-62058DB083E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30260" yWindow="500" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="89">
   <si>
     <t>Lundi</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>E207</t>
+  </si>
+  <si>
+    <t>E209</t>
   </si>
 </sst>
 </file>
@@ -377,6 +380,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29040E5A-5519-964C-B6DE-2A568682510C}" name="Table1" displayName="Table1" ref="A1:I39" totalsRowShown="0">
   <autoFilter ref="A1:I39" xr:uid="{29040E5A-5519-964C-B6DE-2A568682510C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I39">
+    <sortCondition ref="E2:E39"/>
+    <sortCondition ref="A2:A39"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{886CAE80-8B7C-814A-A2B4-5713C370F8E6}" name="day"/>
     <tableColumn id="2" xr3:uid="{7B15CDD9-9A75-8345-ACFD-50613399562F}" name="start_time" dataDxfId="2"/>
@@ -711,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF1DC5-63E0-A14F-8B6A-86AB73F394B2}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,22 +766,22 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -782,28 +789,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -811,7 +818,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
@@ -823,16 +830,16 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -840,7 +847,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -858,7 +865,7 @@
         <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
         <v>56</v>
@@ -869,28 +876,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -898,28 +905,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -927,7 +934,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -939,16 +946,16 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -956,31 +963,31 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -997,16 +1004,16 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1014,86 +1021,86 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1101,25 +1108,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -1130,7 +1137,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1142,16 +1149,16 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1162,25 +1169,25 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1217,7 +1224,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
@@ -1229,16 +1236,16 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -1246,7 +1253,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -1258,19 +1265,19 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1278,25 +1285,25 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
         <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1304,28 +1311,28 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1333,89 +1340,89 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
         <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="H22" t="s">
         <v>37</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2">
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="H24" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1423,25 +1430,25 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25" s="2">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="H25" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1452,57 +1459,57 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="H26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G27" t="s">
         <v>7</v>
       </c>
       <c r="H27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1513,22 +1520,22 @@
         <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -1539,25 +1546,25 @@
         <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H29" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -1568,28 +1575,28 @@
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1606,19 +1613,19 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1635,16 +1642,16 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -1652,13 +1659,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D33" s="2">
         <v>2</v>
@@ -1667,10 +1674,10 @@
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="H33" t="s">
         <v>72</v>
@@ -1681,86 +1688,86 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D34" s="2">
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G34" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" s="2">
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G35" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G36" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I36">
         <v>2</v>
@@ -1768,28 +1775,28 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="2">
         <v>3</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="2">
-        <v>2</v>
-      </c>
       <c r="E37" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -1797,28 +1804,28 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D38" s="2">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F38" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -1829,28 +1836,28 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="H39" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
erreur span mardi seb
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ADCC45-6D95-7F48-A20D-A30E8A6FC2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18AB4A3-AC15-F043-AEA0-596328B97A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="28580" windowHeight="17780" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -335,7 +335,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +705,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C32"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1596,7 +1596,7 @@
         <v>43</v>
       </c>
       <c r="D31" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>29</v>
@@ -1625,7 +1625,7 @@
         <v>44</v>
       </c>
       <c r="D32" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Ajout de Virgil dans horaire
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D766745-9079-AE40-8F9D-A54A2BCBAA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2DCBC3-D351-2A4B-8CF4-205E45E81B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="28580" windowHeight="17780" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="83">
   <si>
     <t>Lundi</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mégadonnées </t>
+  </si>
+  <si>
+    <t>Virgil</t>
+  </si>
+  <si>
+    <t>VD</t>
   </si>
 </sst>
 </file>
@@ -705,7 +711,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
         <v>49</v>
@@ -1260,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1338,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
         <v>71</v>
@@ -1347,7 +1353,7 @@
         <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1425,7 +1431,7 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
         <v>71</v>
@@ -1434,7 +1440,7 @@
         <v>28</v>
       </c>
       <c r="H25" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="I25">
         <v>1</v>

</xml_diff>